<commit_message>
Implement CIC and CICComp manage from stm32
</commit_message>
<xml_diff>
--- a/Scheme/Decimation.xlsx
+++ b/Scheme/Decimation.xlsx
@@ -415,7 +415,7 @@
   <dimension ref="B2:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,7 +447,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="3">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -488,7 +488,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
@@ -496,7 +496,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="3">
-        <v>256</v>
+        <v>2560</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
@@ -508,7 +508,7 @@
       </c>
       <c r="C12" s="4">
         <f>C9/C11</f>
-        <v>480000</v>
+        <v>48000</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
@@ -535,7 +535,7 @@
       </c>
       <c r="C15" s="4">
         <f>C12*C4</f>
-        <v>3360000</v>
+        <v>3072000</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>